<commit_message>
changed names of tenses
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -17213,22 +17213,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="21.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="5" width="25.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="22.37"/>

</xml_diff>